<commit_message>
Arch, need to get gud now
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giajordan\Documents\GitHub\LC-PreProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF93032D-C926-4FF3-AA24-0A7D01AD5C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8827A837-05E9-4CAC-98D2-6B753D1FDD04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{DACB58F3-1851-4104-993D-6C0B9EF056F6}"/>
   </bookViews>
@@ -36,78 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
-    <t>b26166_Z00.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z01.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z02.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z03.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z04.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z05.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z06.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z07.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z08.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z09.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z10.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z11.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z12.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z13.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z14.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z15.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z16.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z17.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z18.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z19.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z20.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z21.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z22.ome</t>
-  </si>
-  <si>
-    <t>b26166_Z23.ome</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -121,6 +49,78 @@
   </si>
   <si>
     <t>y2</t>
+  </si>
+  <si>
+    <t>b26166_Z00.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z01.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z02.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z03.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z04.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z05.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z06.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z07.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z08.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z09.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z10.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z11.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z12.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z13.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z14.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z15.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z16.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z17.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z18.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z19.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z20.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z21.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z22.ome.tif</t>
+  </si>
+  <si>
+    <t>b26166_Z23.ome.tif</t>
   </si>
 </sst>
 </file>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1343BA3-4CF5-47C8-91AB-3170A7B10E53}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,24 +485,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1788</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1806</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1824</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1788</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1854</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1800</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1836</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1800</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1830</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1848</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1878</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1746</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1848</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1854</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1902</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1866</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1878</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1914</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1878</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>1926</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>1878</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1890</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>1956</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>1956</v>

</xml_diff>